<commit_message>
Updated project data sheets
Added efficiency2 and fuel2 to all projects
</commit_message>
<xml_diff>
--- a/projects/puerto_rico_stoch/data/data_A.xlsx
+++ b/projects/puerto_rico_stoch/data/data_A.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BBCF1A1-1434-4345-B423-D6E7928E08F0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45A0A873-8E82-48B8-ACC4-AC29C88F25D0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="941" firstSheet="3" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="6840" windowWidth="29040" windowHeight="15840" tabRatio="941" firstSheet="3" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ref" sheetId="4" r:id="rId1"/>
@@ -25,7 +25,7 @@
     <sheet name="ReserveMargin" sheetId="13" r:id="rId15"/>
     <sheet name="capacityFactorTOD" sheetId="14" r:id="rId16"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +33,10 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -41,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1245" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1249" uniqueCount="227">
   <si>
     <t>connection</t>
   </si>
@@ -713,6 +716,15 @@
   </si>
   <si>
     <t>[fr]</t>
+  </si>
+  <si>
+    <t>Efficiency2</t>
+  </si>
+  <si>
+    <t>fuel2</t>
+  </si>
+  <si>
+    <t>[text2]</t>
   </si>
 </sst>
 </file>
@@ -1145,12 +1157,12 @@
       <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>16</v>
       </c>
@@ -1170,7 +1182,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>65</v>
       </c>
@@ -1190,7 +1202,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>86</v>
       </c>
@@ -1198,7 +1210,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>87</v>
       </c>
@@ -1206,7 +1218,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>88</v>
       </c>
@@ -1217,7 +1229,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>89</v>
       </c>
@@ -1225,7 +1237,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>90</v>
       </c>
@@ -1236,7 +1248,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>91</v>
       </c>
@@ -1244,7 +1256,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>92</v>
       </c>
@@ -1252,7 +1264,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>99</v>
       </c>
@@ -1260,7 +1272,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>100</v>
       </c>
@@ -1274,7 +1286,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>136</v>
       </c>
@@ -1282,7 +1294,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>137</v>
       </c>
@@ -1290,7 +1302,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>138</v>
       </c>
@@ -1298,7 +1310,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>139</v>
       </c>
@@ -1306,7 +1318,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
         <v>140</v>
       </c>
@@ -1314,7 +1326,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
         <v>141</v>
       </c>
@@ -1322,7 +1334,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
         <v>142</v>
       </c>
@@ -1330,7 +1342,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
         <v>143</v>
       </c>
@@ -1338,7 +1350,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
         <v>144</v>
       </c>
@@ -1346,7 +1358,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
         <v>145</v>
       </c>
@@ -1354,7 +1366,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
         <v>171</v>
       </c>
@@ -1362,7 +1374,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
         <v>146</v>
       </c>
@@ -1370,7 +1382,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
         <v>149</v>
       </c>
@@ -1378,7 +1390,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
         <v>196</v>
       </c>
@@ -1386,7 +1398,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A26" t="s">
         <v>220</v>
       </c>
@@ -1421,12 +1433,12 @@
       <selection activeCell="R2" sqref="R2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.69140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>21</v>
       </c>
@@ -1440,7 +1452,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>66</v>
       </c>
@@ -1454,7 +1466,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
         <v>94</v>
       </c>
@@ -1472,24 +1484,25 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
-  <dimension ref="A1:I28"/>
+  <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.4609375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.3046875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.4609375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.23046875" style="29"/>
+    <col min="6" max="6" width="12.84375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.4609375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.53515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.4609375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A1" s="8" t="s">
         <v>24</v>
       </c>
@@ -1503,22 +1516,25 @@
         <v>40</v>
       </c>
       <c r="E1" s="8" t="s">
+        <v>224</v>
+      </c>
+      <c r="F1" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="I1" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="J1" s="8" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A2" s="9" t="s">
         <v>69</v>
       </c>
@@ -1532,22 +1548,25 @@
         <v>71</v>
       </c>
       <c r="E2" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="F2" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="G2" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="H2" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="H2" s="9" t="s">
+      <c r="I2" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="I2" s="9" t="s">
+      <c r="J2" s="9" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A3" s="6" t="s">
         <v>106</v>
       </c>
@@ -1560,19 +1579,20 @@
       <c r="D3" s="9">
         <v>34.799999999999997</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="9"/>
+      <c r="F3" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="F3" s="9"/>
       <c r="G3" s="9"/>
-      <c r="H3" s="6">
+      <c r="H3" s="9"/>
+      <c r="I3" s="6">
         <v>75</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="J3" s="6" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A4" s="6" t="s">
         <v>107</v>
       </c>
@@ -1585,17 +1605,18 @@
       <c r="D4" s="9">
         <v>29.9</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="E4" s="9"/>
+      <c r="F4" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="F4" s="9"/>
       <c r="G4" s="9"/>
-      <c r="H4" s="7">
+      <c r="H4" s="9"/>
+      <c r="I4" s="7">
         <v>50</v>
       </c>
-      <c r="I4" s="7"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J4" s="7"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A5" s="6" t="s">
         <v>108</v>
       </c>
@@ -1608,17 +1629,18 @@
       <c r="D5" s="9">
         <v>40</v>
       </c>
-      <c r="E5" s="9" t="s">
+      <c r="E5" s="9"/>
+      <c r="F5" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="F5" s="9"/>
       <c r="G5" s="9"/>
-      <c r="H5" s="7">
+      <c r="H5" s="9"/>
+      <c r="I5" s="7">
         <v>50</v>
       </c>
-      <c r="I5" s="7"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J5" s="7"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A6" s="6" t="s">
         <v>109</v>
       </c>
@@ -1631,17 +1653,18 @@
       <c r="D6" s="9">
         <v>35.299999999999997</v>
       </c>
-      <c r="E6" s="9" t="s">
+      <c r="E6" s="9"/>
+      <c r="F6" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="F6" s="9"/>
       <c r="G6" s="9"/>
-      <c r="H6" s="7">
+      <c r="H6" s="9"/>
+      <c r="I6" s="7">
         <v>55</v>
       </c>
-      <c r="I6" s="7"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J6" s="7"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A7" s="6" t="s">
         <v>110</v>
       </c>
@@ -1654,17 +1677,18 @@
       <c r="D7" s="9">
         <v>34.6</v>
       </c>
-      <c r="E7" s="9" t="s">
+      <c r="E7" s="9"/>
+      <c r="F7" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="F7" s="9"/>
       <c r="G7" s="9"/>
-      <c r="H7" s="7">
+      <c r="H7" s="9"/>
+      <c r="I7" s="7">
         <v>65</v>
       </c>
-      <c r="I7" s="7"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J7" s="7"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A8" s="6" t="s">
         <v>111</v>
       </c>
@@ -1677,17 +1701,18 @@
       <c r="D8" s="9">
         <v>34.1</v>
       </c>
-      <c r="E8" s="9" t="s">
+      <c r="E8" s="9"/>
+      <c r="F8" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="F8" s="9"/>
       <c r="G8" s="9"/>
-      <c r="H8" s="7">
+      <c r="H8" s="9"/>
+      <c r="I8" s="7">
         <v>65</v>
       </c>
-      <c r="I8" s="7"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J8" s="7"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A9" s="6" t="s">
         <v>112</v>
       </c>
@@ -1700,19 +1725,20 @@
       <c r="D9" s="9">
         <v>36.799999999999997</v>
       </c>
-      <c r="E9" s="9" t="s">
+      <c r="E9" s="9"/>
+      <c r="F9" s="9" t="s">
         <v>140</v>
       </c>
-      <c r="F9" s="9"/>
       <c r="G9" s="9"/>
-      <c r="H9" s="6">
+      <c r="H9" s="9"/>
+      <c r="I9" s="6">
         <v>100</v>
       </c>
-      <c r="I9" s="6" t="s">
+      <c r="J9" s="6" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A10" s="6" t="s">
         <v>113</v>
       </c>
@@ -1725,19 +1751,20 @@
       <c r="D10" s="6">
         <v>19</v>
       </c>
-      <c r="E10" s="9" t="s">
+      <c r="E10" s="6"/>
+      <c r="F10" s="9" t="s">
         <v>195</v>
       </c>
-      <c r="F10" s="9"/>
       <c r="G10" s="9"/>
-      <c r="H10" s="6">
+      <c r="H10" s="9"/>
+      <c r="I10" s="6">
         <v>45</v>
       </c>
-      <c r="I10" s="6" t="s">
+      <c r="J10" s="6" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A11" s="6" t="s">
         <v>114</v>
       </c>
@@ -1750,19 +1777,20 @@
       <c r="D11" s="9">
         <v>45.5</v>
       </c>
-      <c r="E11" s="9" t="s">
+      <c r="E11" s="9"/>
+      <c r="F11" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="F11" s="9"/>
       <c r="G11" s="9"/>
-      <c r="H11" s="6">
+      <c r="H11" s="9"/>
+      <c r="I11" s="6">
         <v>55</v>
       </c>
-      <c r="I11" s="6" t="s">
+      <c r="J11" s="6" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A12" s="6" t="s">
         <v>115</v>
       </c>
@@ -1775,19 +1803,20 @@
       <c r="D12" s="6">
         <v>36.799999999999997</v>
       </c>
-      <c r="E12" s="9" t="s">
+      <c r="E12" s="6"/>
+      <c r="F12" s="9" t="s">
         <v>195</v>
       </c>
-      <c r="F12" s="9"/>
       <c r="G12" s="9"/>
-      <c r="H12" s="6">
+      <c r="H12" s="9"/>
+      <c r="I12" s="6">
         <v>30</v>
       </c>
-      <c r="I12" s="9" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J12" s="9" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A13" s="6" t="s">
         <v>116</v>
       </c>
@@ -1800,19 +1829,20 @@
       <c r="D13" s="6">
         <v>36.799999999999997</v>
       </c>
-      <c r="E13" s="9" t="s">
+      <c r="E13" s="6"/>
+      <c r="F13" s="9" t="s">
         <v>195</v>
       </c>
-      <c r="F13" s="9"/>
       <c r="G13" s="9"/>
-      <c r="H13" s="6">
+      <c r="H13" s="9"/>
+      <c r="I13" s="6">
         <v>30</v>
       </c>
-      <c r="I13" s="9" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J13" s="9" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A14" s="22" t="s">
         <v>117</v>
       </c>
@@ -1823,19 +1853,20 @@
       <c r="D14" s="22">
         <v>85</v>
       </c>
-      <c r="E14" s="22" t="s">
-        <v>196</v>
-      </c>
-      <c r="F14" s="22"/>
+      <c r="E14" s="22"/>
+      <c r="F14" s="22" t="s">
+        <v>196</v>
+      </c>
       <c r="G14" s="22"/>
-      <c r="H14" s="22">
+      <c r="H14" s="22"/>
+      <c r="I14" s="22">
         <v>15</v>
       </c>
-      <c r="I14" s="22" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J14" s="22" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A15" s="22" t="s">
         <v>118</v>
       </c>
@@ -1848,19 +1879,20 @@
       <c r="D15" s="22">
         <v>25.3</v>
       </c>
-      <c r="E15" s="22" t="s">
-        <v>196</v>
-      </c>
-      <c r="F15" s="22"/>
+      <c r="E15" s="22"/>
+      <c r="F15" s="22" t="s">
+        <v>196</v>
+      </c>
       <c r="G15" s="22"/>
-      <c r="H15" s="23">
+      <c r="H15" s="22"/>
+      <c r="I15" s="23">
         <v>45</v>
       </c>
-      <c r="I15" s="22" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J15" s="22" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A16" s="22" t="s">
         <v>215</v>
       </c>
@@ -1873,19 +1905,20 @@
       <c r="D16" s="25">
         <v>38.799999999999997</v>
       </c>
-      <c r="E16" s="22" t="s">
-        <v>196</v>
-      </c>
-      <c r="F16" s="22"/>
+      <c r="E16" s="25"/>
+      <c r="F16" s="22" t="s">
+        <v>196</v>
+      </c>
       <c r="G16" s="22"/>
-      <c r="H16" s="22">
+      <c r="H16" s="22"/>
+      <c r="I16" s="22">
         <v>75</v>
       </c>
-      <c r="I16" s="22" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J16" s="22" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A17" s="22" t="s">
         <v>216</v>
       </c>
@@ -1898,19 +1931,20 @@
       <c r="D17" s="25">
         <v>51.7</v>
       </c>
-      <c r="E17" s="22" t="s">
-        <v>196</v>
-      </c>
-      <c r="F17" s="22"/>
+      <c r="E17" s="25"/>
+      <c r="F17" s="22" t="s">
+        <v>196</v>
+      </c>
       <c r="G17" s="22"/>
-      <c r="H17" s="22">
+      <c r="H17" s="22"/>
+      <c r="I17" s="22">
         <v>55</v>
       </c>
-      <c r="I17" s="22" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J17" s="22" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A18" s="22" t="s">
         <v>218</v>
       </c>
@@ -1923,19 +1957,20 @@
       <c r="D18" s="25">
         <v>51.7</v>
       </c>
-      <c r="E18" s="22" t="s">
-        <v>196</v>
-      </c>
-      <c r="F18" s="22"/>
+      <c r="E18" s="25"/>
+      <c r="F18" s="22" t="s">
+        <v>196</v>
+      </c>
       <c r="G18" s="22"/>
-      <c r="H18" s="22">
+      <c r="H18" s="22"/>
+      <c r="I18" s="22">
         <v>55</v>
       </c>
-      <c r="I18" s="22" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J18" s="22" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A19" s="22" t="s">
         <v>119</v>
       </c>
@@ -1948,19 +1983,20 @@
       <c r="D19" s="22">
         <v>62.12</v>
       </c>
-      <c r="E19" s="22" t="s">
-        <v>149</v>
-      </c>
-      <c r="F19" s="22"/>
+      <c r="E19" s="22"/>
+      <c r="F19" s="22" t="s">
+        <v>149</v>
+      </c>
       <c r="G19" s="22"/>
-      <c r="H19" s="22">
+      <c r="H19" s="22"/>
+      <c r="I19" s="22">
         <v>55</v>
       </c>
-      <c r="I19" s="22" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J19" s="22" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A20" s="22" t="s">
         <v>120</v>
       </c>
@@ -1973,19 +2009,20 @@
       <c r="D20" s="22">
         <v>42.34</v>
       </c>
-      <c r="E20" s="22" t="s">
-        <v>149</v>
-      </c>
-      <c r="F20" s="22"/>
+      <c r="E20" s="22"/>
+      <c r="F20" s="22" t="s">
+        <v>149</v>
+      </c>
       <c r="G20" s="22"/>
-      <c r="H20" s="23">
+      <c r="H20" s="22"/>
+      <c r="I20" s="23">
         <v>55</v>
       </c>
-      <c r="I20" s="22" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J20" s="22" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A21" s="22" t="s">
         <v>121</v>
       </c>
@@ -1998,19 +2035,20 @@
       <c r="D21" s="22">
         <v>36.799999999999997</v>
       </c>
-      <c r="E21" s="22" t="s">
+      <c r="E21" s="22"/>
+      <c r="F21" s="22" t="s">
         <v>195</v>
       </c>
-      <c r="F21" s="22"/>
       <c r="G21" s="22"/>
-      <c r="H21" s="22">
+      <c r="H21" s="22"/>
+      <c r="I21" s="22">
         <v>30</v>
       </c>
-      <c r="I21" s="22" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J21" s="22" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A22" s="22" t="s">
         <v>122</v>
       </c>
@@ -2023,19 +2061,20 @@
       <c r="D22" s="22">
         <v>36.799999999999997</v>
       </c>
-      <c r="E22" s="22" t="s">
+      <c r="E22" s="22"/>
+      <c r="F22" s="22" t="s">
         <v>195</v>
       </c>
-      <c r="F22" s="22"/>
       <c r="G22" s="22"/>
-      <c r="H22" s="22">
+      <c r="H22" s="22"/>
+      <c r="I22" s="22">
         <v>30</v>
       </c>
-      <c r="I22" s="22" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J22" s="22" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A23" s="6" t="s">
         <v>131</v>
       </c>
@@ -2046,19 +2085,20 @@
       <c r="D23" s="9">
         <v>85</v>
       </c>
-      <c r="E23" s="9" t="s">
-        <v>196</v>
-      </c>
-      <c r="F23" s="9"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="9" t="s">
+        <v>196</v>
+      </c>
       <c r="G23" s="9"/>
-      <c r="H23" s="9">
+      <c r="H23" s="9"/>
+      <c r="I23" s="9">
         <v>15</v>
       </c>
-      <c r="I23" s="9" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J23" s="9" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A24" s="6" t="s">
         <v>132</v>
       </c>
@@ -2071,19 +2111,20 @@
       <c r="D24" s="6">
         <v>25.3</v>
       </c>
-      <c r="E24" s="9" t="s">
-        <v>196</v>
-      </c>
-      <c r="F24" s="6"/>
-      <c r="G24" s="9"/>
-      <c r="H24" s="9">
+      <c r="E24" s="6"/>
+      <c r="F24" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="G24" s="6"/>
+      <c r="H24" s="9"/>
+      <c r="I24" s="9">
         <v>45</v>
       </c>
-      <c r="I24" s="9" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J24" s="9" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A25" s="6" t="s">
         <v>194</v>
       </c>
@@ -2096,19 +2137,20 @@
       <c r="D25" s="9">
         <v>54.17</v>
       </c>
-      <c r="E25" s="6" t="s">
-        <v>149</v>
-      </c>
-      <c r="F25" s="6"/>
-      <c r="G25" s="9"/>
-      <c r="H25" s="6">
+      <c r="E25" s="9"/>
+      <c r="F25" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="G25" s="6"/>
+      <c r="H25" s="9"/>
+      <c r="I25" s="6">
         <v>55</v>
       </c>
-      <c r="I25" s="9" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J25" s="9" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A26" s="6" t="s">
         <v>133</v>
       </c>
@@ -2121,19 +2163,20 @@
       <c r="D26" s="9">
         <v>37.11</v>
       </c>
-      <c r="E26" s="6" t="s">
-        <v>149</v>
-      </c>
-      <c r="F26" s="6"/>
-      <c r="G26" s="9"/>
-      <c r="H26" s="9">
+      <c r="E26" s="9"/>
+      <c r="F26" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="G26" s="6"/>
+      <c r="H26" s="9"/>
+      <c r="I26" s="9">
         <v>55</v>
       </c>
-      <c r="I26" s="9" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J26" s="9" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A27" s="6" t="s">
         <v>134</v>
       </c>
@@ -2146,19 +2189,20 @@
       <c r="D27" s="6">
         <v>36.799999999999997</v>
       </c>
-      <c r="E27" s="9" t="s">
+      <c r="E27" s="6"/>
+      <c r="F27" s="9" t="s">
         <v>195</v>
       </c>
-      <c r="F27" s="6"/>
-      <c r="G27" s="9"/>
-      <c r="H27" s="9">
+      <c r="G27" s="6"/>
+      <c r="H27" s="9"/>
+      <c r="I27" s="9">
         <v>30</v>
       </c>
-      <c r="I27" s="9" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J27" s="9" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A28" s="6" t="s">
         <v>135</v>
       </c>
@@ -2171,15 +2215,16 @@
       <c r="D28" s="6">
         <v>36.799999999999997</v>
       </c>
-      <c r="E28" s="9" t="s">
+      <c r="E28" s="6"/>
+      <c r="F28" s="9" t="s">
         <v>195</v>
       </c>
-      <c r="F28" s="6"/>
-      <c r="G28" s="9"/>
-      <c r="H28" s="9">
+      <c r="G28" s="6"/>
+      <c r="H28" s="9"/>
+      <c r="I28" s="9">
         <v>30</v>
       </c>
-      <c r="I28" s="9" t="s">
+      <c r="J28" s="9" t="s">
         <v>196</v>
       </c>
     </row>
@@ -2197,18 +2242,18 @@
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.109375" customWidth="1"/>
+    <col min="1" max="1" width="10.3046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.53515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.4609375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.69140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.3046875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.3046875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.07421875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>24</v>
       </c>
@@ -2231,7 +2276,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>66</v>
       </c>
@@ -2254,7 +2299,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A3" s="6" t="s">
         <v>106</v>
       </c>
@@ -2273,7 +2318,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A4" s="6" t="s">
         <v>107</v>
       </c>
@@ -2292,7 +2337,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A5" s="6" t="s">
         <v>108</v>
       </c>
@@ -2311,7 +2356,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A6" s="6" t="s">
         <v>109</v>
       </c>
@@ -2330,7 +2375,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A7" s="6" t="s">
         <v>110</v>
       </c>
@@ -2349,7 +2394,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A8" s="6" t="s">
         <v>111</v>
       </c>
@@ -2368,7 +2413,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A9" s="6" t="s">
         <v>112</v>
       </c>
@@ -2391,7 +2436,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A10" s="6" t="s">
         <v>113</v>
       </c>
@@ -2410,7 +2455,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A11" s="6" t="s">
         <v>114</v>
       </c>
@@ -2429,7 +2474,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A12" s="6" t="s">
         <v>115</v>
       </c>
@@ -2448,7 +2493,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A13" s="6" t="s">
         <v>116</v>
       </c>
@@ -2467,7 +2512,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A14" s="22" t="s">
         <v>117</v>
       </c>
@@ -2490,7 +2535,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A15" s="22" t="s">
         <v>118</v>
       </c>
@@ -2513,7 +2558,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A16" s="22" t="s">
         <v>215</v>
       </c>
@@ -2536,7 +2581,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A17" s="22" t="s">
         <v>216</v>
       </c>
@@ -2557,7 +2602,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A18" s="22" t="s">
         <v>218</v>
       </c>
@@ -2578,7 +2623,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A19" s="22" t="s">
         <v>119</v>
       </c>
@@ -2601,7 +2646,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A20" s="22" t="s">
         <v>120</v>
       </c>
@@ -2624,7 +2669,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A21" s="22" t="s">
         <v>121</v>
       </c>
@@ -2647,7 +2692,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A22" s="22" t="s">
         <v>122</v>
       </c>
@@ -2670,7 +2715,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A23" s="6" t="s">
         <v>131</v>
       </c>
@@ -2693,7 +2738,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A24" s="6" t="s">
         <v>132</v>
       </c>
@@ -2716,7 +2761,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A25" s="6" t="s">
         <v>194</v>
       </c>
@@ -2739,7 +2784,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A26" s="6" t="s">
         <v>133</v>
       </c>
@@ -2762,7 +2807,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A27" s="6" t="s">
         <v>134</v>
       </c>
@@ -2785,7 +2830,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A28" s="6" t="s">
         <v>135</v>
       </c>
@@ -2808,7 +2853,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.4">
       <c r="F29" s="7"/>
       <c r="G29" s="6"/>
       <c r="H29" s="6"/>
@@ -2828,18 +2873,18 @@
       <selection activeCell="F21" sqref="F21:F28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.3046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.4609375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.3046875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.53515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.4609375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.53515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.4609375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>24</v>
       </c>
@@ -2862,7 +2907,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>66</v>
       </c>
@@ -2885,7 +2930,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A3" s="6" t="s">
         <v>106</v>
       </c>
@@ -2896,7 +2941,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A4" s="6" t="s">
         <v>107</v>
       </c>
@@ -2907,7 +2952,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A5" s="6" t="s">
         <v>108</v>
       </c>
@@ -2918,7 +2963,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A6" s="6" t="s">
         <v>109</v>
       </c>
@@ -2929,7 +2974,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A7" s="6" t="s">
         <v>110</v>
       </c>
@@ -2940,7 +2985,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A8" s="6" t="s">
         <v>111</v>
       </c>
@@ -2951,7 +2996,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A9" s="6" t="s">
         <v>112</v>
       </c>
@@ -2964,35 +3009,35 @@
         <v>143</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A10" s="6" t="s">
         <v>113</v>
       </c>
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A11" s="6" t="s">
         <v>114</v>
       </c>
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A12" s="6" t="s">
         <v>115</v>
       </c>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A13" s="6" t="s">
         <v>116</v>
       </c>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A14" s="22" t="s">
         <v>117</v>
       </c>
@@ -3003,7 +3048,7 @@
       <c r="F14" s="25"/>
       <c r="G14" s="25"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A15" s="22" t="s">
         <v>118</v>
       </c>
@@ -3018,7 +3063,7 @@
       <c r="F15" s="25"/>
       <c r="G15" s="25"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A16" s="22" t="s">
         <v>215</v>
       </c>
@@ -3033,7 +3078,7 @@
       <c r="F16" s="25"/>
       <c r="G16" s="25"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A17" s="22" t="s">
         <v>216</v>
       </c>
@@ -3048,7 +3093,7 @@
       <c r="F17" s="25"/>
       <c r="G17" s="25"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A18" s="22" t="s">
         <v>218</v>
       </c>
@@ -3063,7 +3108,7 @@
       <c r="F18" s="25"/>
       <c r="G18" s="25"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A19" s="22" t="s">
         <v>119</v>
       </c>
@@ -3078,7 +3123,7 @@
       <c r="F19" s="25"/>
       <c r="G19" s="25"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A20" s="22" t="s">
         <v>120</v>
       </c>
@@ -3089,7 +3134,7 @@
       <c r="F20" s="25"/>
       <c r="G20" s="25"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A21" s="22" t="s">
         <v>121</v>
       </c>
@@ -3102,7 +3147,7 @@
       </c>
       <c r="G21" s="25"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A22" s="22" t="s">
         <v>122</v>
       </c>
@@ -3115,12 +3160,12 @@
       </c>
       <c r="G22" s="25"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A23" s="6" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A24" s="6" t="s">
         <v>132</v>
       </c>
@@ -3131,7 +3176,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A25" s="6" t="s">
         <v>194</v>
       </c>
@@ -3142,12 +3187,12 @@
         <v>136</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A26" s="6" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A27" s="6" t="s">
         <v>134</v>
       </c>
@@ -3155,7 +3200,7 @@
         <v>738</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A28" s="6" t="s">
         <v>135</v>
       </c>
@@ -3177,14 +3222,14 @@
       <selection activeCell="M30" sqref="M30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.69140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.3046875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.69140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>24</v>
       </c>
@@ -3198,7 +3243,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>66</v>
       </c>
@@ -3212,7 +3257,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A3" s="6" t="s">
         <v>106</v>
       </c>
@@ -3226,7 +3271,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A4" s="6" t="s">
         <v>107</v>
       </c>
@@ -3240,7 +3285,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A5" s="6" t="s">
         <v>107</v>
       </c>
@@ -3254,7 +3299,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A6" s="6" t="s">
         <v>107</v>
       </c>
@@ -3268,7 +3313,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A7" s="6" t="s">
         <v>108</v>
       </c>
@@ -3282,7 +3327,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A8" s="6" t="s">
         <v>108</v>
       </c>
@@ -3296,7 +3341,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A9" s="6" t="s">
         <v>108</v>
       </c>
@@ -3310,7 +3355,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A10" s="6" t="s">
         <v>109</v>
       </c>
@@ -3324,7 +3369,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A11" s="6" t="s">
         <v>110</v>
       </c>
@@ -3338,7 +3383,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A12" s="6" t="s">
         <v>110</v>
       </c>
@@ -3352,7 +3397,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A13" s="6" t="s">
         <v>110</v>
       </c>
@@ -3366,7 +3411,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A14" s="6" t="s">
         <v>110</v>
       </c>
@@ -3380,7 +3425,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A15" s="6" t="s">
         <v>111</v>
       </c>
@@ -3394,7 +3439,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A16" s="6" t="s">
         <v>111</v>
       </c>
@@ -3408,7 +3453,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A17" s="6" t="s">
         <v>111</v>
       </c>
@@ -3422,7 +3467,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A18" s="6" t="s">
         <v>111</v>
       </c>
@@ -3436,7 +3481,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A19" s="6" t="s">
         <v>111</v>
       </c>
@@ -3450,7 +3495,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A20" s="6" t="s">
         <v>111</v>
       </c>
@@ -3464,7 +3509,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A21" s="6" t="s">
         <v>112</v>
       </c>
@@ -3478,7 +3523,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A22" s="6" t="s">
         <v>113</v>
       </c>
@@ -3492,7 +3537,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A23" s="6" t="s">
         <v>114</v>
       </c>
@@ -3506,7 +3551,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A24" s="6" t="s">
         <v>115</v>
       </c>
@@ -3520,7 +3565,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A25" s="6" t="s">
         <v>115</v>
       </c>
@@ -3534,7 +3579,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A26" s="6" t="s">
         <v>116</v>
       </c>
@@ -3562,14 +3607,14 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.3046875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.109375" customWidth="1"/>
+    <col min="3" max="3" width="9.07421875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>46</v>
       </c>
@@ -3577,7 +3622,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>82</v>
       </c>
@@ -3585,7 +3630,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A3">
         <v>0.36215000000000003</v>
       </c>
@@ -3599,19 +3644,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:E98"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F1" sqref="F1:I1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.3046875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.53515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.69140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>21</v>
       </c>
@@ -3628,7 +3673,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>66</v>
       </c>
@@ -3645,7 +3690,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A3" s="3" t="s">
         <v>95</v>
       </c>
@@ -3662,7 +3707,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A4" s="3" t="s">
         <v>95</v>
       </c>
@@ -3679,7 +3724,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A5" s="3" t="s">
         <v>95</v>
       </c>
@@ -3696,7 +3741,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A6" s="3" t="s">
         <v>95</v>
       </c>
@@ -3713,7 +3758,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A7" s="3" t="s">
         <v>95</v>
       </c>
@@ -3730,7 +3775,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A8" s="3" t="s">
         <v>95</v>
       </c>
@@ -3747,7 +3792,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A9" s="3" t="s">
         <v>95</v>
       </c>
@@ -3764,7 +3809,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A10" s="3" t="s">
         <v>95</v>
       </c>
@@ -3781,7 +3826,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A11" s="3" t="s">
         <v>95</v>
       </c>
@@ -3798,7 +3843,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A12" s="3" t="s">
         <v>95</v>
       </c>
@@ -3815,7 +3860,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A13" s="3" t="s">
         <v>95</v>
       </c>
@@ -3832,7 +3877,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A14" s="3" t="s">
         <v>95</v>
       </c>
@@ -3849,7 +3894,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A15" s="3" t="s">
         <v>95</v>
       </c>
@@ -3866,7 +3911,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A16" s="3" t="s">
         <v>95</v>
       </c>
@@ -3883,7 +3928,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A17" s="3" t="s">
         <v>95</v>
       </c>
@@ -3900,7 +3945,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A18" s="3" t="s">
         <v>95</v>
       </c>
@@ -3917,7 +3962,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A19" s="3" t="s">
         <v>95</v>
       </c>
@@ -3934,7 +3979,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A20" s="3" t="s">
         <v>95</v>
       </c>
@@ -3951,7 +3996,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A21" s="3" t="s">
         <v>95</v>
       </c>
@@ -3968,7 +4013,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A22" s="3" t="s">
         <v>95</v>
       </c>
@@ -3985,7 +4030,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A23" s="3" t="s">
         <v>95</v>
       </c>
@@ -4002,7 +4047,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A24" s="3" t="s">
         <v>95</v>
       </c>
@@ -4019,7 +4064,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A25" s="3" t="s">
         <v>95</v>
       </c>
@@ -4036,7 +4081,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A26" s="3" t="s">
         <v>95</v>
       </c>
@@ -4053,7 +4098,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A27" s="3" t="s">
         <v>95</v>
       </c>
@@ -4070,7 +4115,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A28" s="3" t="s">
         <v>95</v>
       </c>
@@ -4087,7 +4132,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A29" s="3" t="s">
         <v>95</v>
       </c>
@@ -4104,7 +4149,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A30" s="3" t="s">
         <v>95</v>
       </c>
@@ -4121,7 +4166,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A31" s="3" t="s">
         <v>95</v>
       </c>
@@ -4138,7 +4183,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A32" s="3" t="s">
         <v>95</v>
       </c>
@@ -4155,7 +4200,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A33" s="3" t="s">
         <v>95</v>
       </c>
@@ -4172,7 +4217,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A34" s="3" t="s">
         <v>95</v>
       </c>
@@ -4189,7 +4234,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A35" s="3" t="s">
         <v>95</v>
       </c>
@@ -4206,7 +4251,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A36" s="3" t="s">
         <v>95</v>
       </c>
@@ -4223,7 +4268,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A37" s="3" t="s">
         <v>95</v>
       </c>
@@ -4240,7 +4285,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A38" s="3" t="s">
         <v>95</v>
       </c>
@@ -4257,7 +4302,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A39" s="3" t="s">
         <v>95</v>
       </c>
@@ -4274,7 +4319,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A40" s="3" t="s">
         <v>95</v>
       </c>
@@ -4291,7 +4336,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A41" s="3" t="s">
         <v>95</v>
       </c>
@@ -4308,7 +4353,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A42" s="3" t="s">
         <v>95</v>
       </c>
@@ -4325,7 +4370,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A43" s="3" t="s">
         <v>95</v>
       </c>
@@ -4342,7 +4387,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A44" s="3" t="s">
         <v>95</v>
       </c>
@@ -4359,7 +4404,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A45" s="3" t="s">
         <v>95</v>
       </c>
@@ -4376,7 +4421,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A46" s="3" t="s">
         <v>95</v>
       </c>
@@ -4393,7 +4438,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A47" s="3" t="s">
         <v>95</v>
       </c>
@@ -4410,7 +4455,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A48" s="3" t="s">
         <v>95</v>
       </c>
@@ -4427,7 +4472,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A49" s="3" t="s">
         <v>95</v>
       </c>
@@ -4444,7 +4489,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A50" s="3" t="s">
         <v>95</v>
       </c>
@@ -4461,7 +4506,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A51" s="3" t="s">
         <v>96</v>
       </c>
@@ -4478,7 +4523,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A52" s="3" t="s">
         <v>96</v>
       </c>
@@ -4495,7 +4540,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A53" s="3" t="s">
         <v>96</v>
       </c>
@@ -4512,7 +4557,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A54" s="3" t="s">
         <v>96</v>
       </c>
@@ -4529,7 +4574,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A55" s="3" t="s">
         <v>96</v>
       </c>
@@ -4546,7 +4591,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A56" s="3" t="s">
         <v>96</v>
       </c>
@@ -4563,7 +4608,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A57" s="3" t="s">
         <v>96</v>
       </c>
@@ -4580,7 +4625,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A58" s="3" t="s">
         <v>96</v>
       </c>
@@ -4597,7 +4642,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A59" s="3" t="s">
         <v>96</v>
       </c>
@@ -4614,7 +4659,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A60" s="3" t="s">
         <v>96</v>
       </c>
@@ -4631,7 +4676,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A61" s="3" t="s">
         <v>96</v>
       </c>
@@ -4648,7 +4693,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A62" s="3" t="s">
         <v>96</v>
       </c>
@@ -4665,7 +4710,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A63" s="3" t="s">
         <v>96</v>
       </c>
@@ -4682,7 +4727,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A64" s="3" t="s">
         <v>96</v>
       </c>
@@ -4699,7 +4744,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A65" s="3" t="s">
         <v>96</v>
       </c>
@@ -4716,7 +4761,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A66" s="3" t="s">
         <v>96</v>
       </c>
@@ -4733,7 +4778,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A67" s="3" t="s">
         <v>96</v>
       </c>
@@ -4750,7 +4795,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A68" s="3" t="s">
         <v>96</v>
       </c>
@@ -4767,7 +4812,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A69" s="3" t="s">
         <v>96</v>
       </c>
@@ -4784,7 +4829,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A70" s="3" t="s">
         <v>96</v>
       </c>
@@ -4801,7 +4846,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A71" s="3" t="s">
         <v>96</v>
       </c>
@@ -4818,7 +4863,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A72" s="3" t="s">
         <v>96</v>
       </c>
@@ -4835,7 +4880,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A73" s="3" t="s">
         <v>96</v>
       </c>
@@ -4852,7 +4897,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A74" s="3" t="s">
         <v>96</v>
       </c>
@@ -4869,7 +4914,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A75" s="3" t="s">
         <v>96</v>
       </c>
@@ -4886,7 +4931,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A76" s="3" t="s">
         <v>96</v>
       </c>
@@ -4903,7 +4948,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A77" s="3" t="s">
         <v>96</v>
       </c>
@@ -4920,7 +4965,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A78" s="3" t="s">
         <v>96</v>
       </c>
@@ -4937,7 +4982,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A79" s="3" t="s">
         <v>96</v>
       </c>
@@ -4954,7 +4999,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A80" s="3" t="s">
         <v>96</v>
       </c>
@@ -4971,7 +5016,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A81" s="3" t="s">
         <v>96</v>
       </c>
@@ -4988,7 +5033,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A82" s="3" t="s">
         <v>96</v>
       </c>
@@ -5005,7 +5050,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A83" s="3" t="s">
         <v>96</v>
       </c>
@@ -5022,7 +5067,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A84" s="3" t="s">
         <v>96</v>
       </c>
@@ -5039,7 +5084,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A85" s="3" t="s">
         <v>96</v>
       </c>
@@ -5056,7 +5101,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A86" s="3" t="s">
         <v>96</v>
       </c>
@@ -5073,7 +5118,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A87" s="3" t="s">
         <v>96</v>
       </c>
@@ -5090,7 +5135,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A88" s="3" t="s">
         <v>96</v>
       </c>
@@ -5107,7 +5152,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A89" s="3" t="s">
         <v>96</v>
       </c>
@@ -5124,7 +5169,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A90" s="3" t="s">
         <v>96</v>
       </c>
@@ -5141,7 +5186,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A91" s="3" t="s">
         <v>96</v>
       </c>
@@ -5158,7 +5203,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A92" s="3" t="s">
         <v>96</v>
       </c>
@@ -5175,7 +5220,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A93" s="3" t="s">
         <v>96</v>
       </c>
@@ -5192,7 +5237,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A94" s="3" t="s">
         <v>96</v>
       </c>
@@ -5209,7 +5254,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A95" s="3" t="s">
         <v>96</v>
       </c>
@@ -5226,7 +5271,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A96" s="3" t="s">
         <v>96</v>
       </c>
@@ -5243,7 +5288,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A97" s="3" t="s">
         <v>96</v>
       </c>
@@ -5260,7 +5305,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A98" s="3" t="s">
         <v>96</v>
       </c>
@@ -5289,13 +5334,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="16.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.4609375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.69140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>48</v>
       </c>
@@ -5306,7 +5351,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>70</v>
       </c>
@@ -5317,7 +5362,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>83</v>
       </c>
@@ -5328,7 +5373,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>84</v>
       </c>
@@ -5352,13 +5397,13 @@
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.69140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.69140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>64</v>
       </c>
@@ -5369,7 +5414,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>70</v>
       </c>
@@ -5380,7 +5425,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>185</v>
       </c>
@@ -5391,7 +5436,7 @@
         <v>4.1667000000000003E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>186</v>
       </c>
@@ -5402,7 +5447,7 @@
         <v>4.1667000000000003E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>187</v>
       </c>
@@ -5413,7 +5458,7 @@
         <v>4.1667000000000003E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>188</v>
       </c>
@@ -5424,7 +5469,7 @@
         <v>4.1667000000000003E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>189</v>
       </c>
@@ -5435,7 +5480,7 @@
         <v>4.1667000000000003E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>190</v>
       </c>
@@ -5446,7 +5491,7 @@
         <v>4.1667000000000003E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>191</v>
       </c>
@@ -5457,7 +5502,7 @@
         <v>4.1667000000000003E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>192</v>
       </c>
@@ -5468,7 +5513,7 @@
         <v>4.1667000000000003E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>193</v>
       </c>
@@ -5479,7 +5524,7 @@
         <v>4.1667000000000003E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>49</v>
       </c>
@@ -5490,7 +5535,7 @@
         <v>4.1667000000000003E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>50</v>
       </c>
@@ -5501,7 +5546,7 @@
         <v>4.1667000000000003E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>51</v>
       </c>
@@ -5512,7 +5557,7 @@
         <v>4.1667000000000003E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>52</v>
       </c>
@@ -5523,7 +5568,7 @@
         <v>4.1667000000000003E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
         <v>53</v>
       </c>
@@ -5534,7 +5579,7 @@
         <v>4.1667000000000003E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
         <v>54</v>
       </c>
@@ -5545,7 +5590,7 @@
         <v>4.1667000000000003E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
         <v>55</v>
       </c>
@@ -5556,7 +5601,7 @@
         <v>4.1667000000000003E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
         <v>56</v>
       </c>
@@ -5567,7 +5612,7 @@
         <v>4.1667000000000003E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
         <v>57</v>
       </c>
@@ -5578,7 +5623,7 @@
         <v>4.1667000000000003E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
         <v>58</v>
       </c>
@@ -5589,7 +5634,7 @@
         <v>4.1667000000000003E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
         <v>59</v>
       </c>
@@ -5600,7 +5645,7 @@
         <v>4.1667000000000003E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
         <v>60</v>
       </c>
@@ -5611,7 +5656,7 @@
         <v>4.1667000000000003E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
         <v>61</v>
       </c>
@@ -5622,7 +5667,7 @@
         <v>4.1667000000000003E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
         <v>62</v>
       </c>
@@ -5633,7 +5678,7 @@
         <v>4.1667000000000003E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A26" t="s">
         <v>85</v>
       </c>
@@ -5658,19 +5703,19 @@
       <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.109375" customWidth="1"/>
+    <col min="1" max="1" width="12.69140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="13.53515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.3046875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.3046875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.53515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.4609375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.4609375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.07421875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -5705,7 +5750,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>70</v>
       </c>
@@ -5740,7 +5785,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>101</v>
       </c>
@@ -5775,7 +5820,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>197</v>
       </c>
@@ -5806,7 +5851,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>202</v>
       </c>
@@ -5841,7 +5886,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>203</v>
       </c>
@@ -5876,7 +5921,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>103</v>
       </c>
@@ -5896,7 +5941,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>201</v>
       </c>
@@ -5931,7 +5976,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>200</v>
       </c>
@@ -5966,7 +6011,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>205</v>
       </c>
@@ -5989,7 +6034,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>206</v>
       </c>
@@ -6012,7 +6057,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>213</v>
       </c>
@@ -6035,7 +6080,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>207</v>
       </c>
@@ -6058,7 +6103,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>208</v>
       </c>
@@ -6095,13 +6140,13 @@
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.07421875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.69140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -6115,7 +6160,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>66</v>
       </c>
@@ -6129,7 +6174,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>101</v>
       </c>
@@ -6143,7 +6188,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>197</v>
       </c>
@@ -6157,7 +6202,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>203</v>
       </c>
@@ -6171,7 +6216,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>202</v>
       </c>
@@ -6199,12 +6244,12 @@
       <selection activeCell="Q6" sqref="Q6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="3" max="3" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.84375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>13</v>
       </c>
@@ -6218,7 +6263,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>67</v>
       </c>
@@ -6232,7 +6277,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A3">
         <v>2016</v>
       </c>
@@ -6246,7 +6291,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A4">
         <v>2021</v>
       </c>
@@ -6260,7 +6305,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A5">
         <v>2026</v>
       </c>
@@ -6274,7 +6319,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A6">
         <v>2031</v>
       </c>
@@ -6288,7 +6333,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A7">
         <v>2036</v>
       </c>
@@ -6302,7 +6347,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A8">
         <v>2041</v>
       </c>
@@ -6330,13 +6375,13 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.07421875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.53515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>80</v>
       </c>
@@ -6344,7 +6389,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>82</v>
       </c>
@@ -6352,7 +6397,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A3">
         <v>0.09</v>
       </c>
@@ -6373,21 +6418,21 @@
       <selection activeCell="D3" sqref="D3:D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.69140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.53515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.4609375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.84375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.69140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.69140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.69140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.69140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.69140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.53515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>21</v>
       </c>
@@ -6425,7 +6470,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>70</v>
       </c>
@@ -6463,7 +6508,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>123</v>
       </c>
@@ -6490,7 +6535,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>98</v>
       </c>
@@ -6520,7 +6565,7 @@
       </c>
       <c r="L4" s="1"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>124</v>
       </c>
@@ -6549,7 +6594,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>97</v>
       </c>
@@ -6563,7 +6608,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>126</v>
       </c>
@@ -6583,7 +6628,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>125</v>
       </c>
@@ -6612,7 +6657,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>94</v>
       </c>
@@ -6644,7 +6689,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>95</v>
       </c>
@@ -6658,7 +6703,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>96</v>
       </c>
@@ -6680,20 +6725,21 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="A1:I28"/>
+  <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I29" sqref="I29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.69140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.3046875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.3046875" style="29" customWidth="1"/>
+    <col min="4" max="4" width="12.53515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A1" s="5" t="s">
         <v>24</v>
       </c>
@@ -6701,28 +6747,31 @@
         <v>21</v>
       </c>
       <c r="C1" s="5" t="s">
+        <v>225</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>182</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A2" s="6" t="s">
         <v>70</v>
       </c>
@@ -6730,10 +6779,10 @@
         <v>66</v>
       </c>
       <c r="C2" s="6" t="s">
+        <v>226</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>66</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>78</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>78</v>
@@ -6748,780 +6797,809 @@
         <v>78</v>
       </c>
       <c r="I2" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="J2" s="6" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A3" s="6" t="s">
         <v>106</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>210</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="6"/>
+      <c r="D3" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="E3" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="E3" s="29" t="s">
+      <c r="F3" s="29" t="s">
         <v>130</v>
       </c>
-      <c r="F3" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="7" t="s">
         <v>129</v>
       </c>
       <c r="H3" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="J3">
         <v>0.9</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A4" s="6" t="s">
         <v>107</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>209</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="6"/>
+      <c r="D4" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="E4" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="E4" s="29" t="s">
+      <c r="F4" s="29" t="s">
         <v>130</v>
       </c>
-      <c r="F4" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="G4" s="6" t="s">
+      <c r="G4" s="7" t="s">
         <v>129</v>
       </c>
       <c r="H4" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="J4">
         <v>0.91</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A5" s="6" t="s">
         <v>108</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>209</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="6"/>
+      <c r="D5" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="E5" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="E5" s="29" t="s">
+      <c r="F5" s="29" t="s">
         <v>130</v>
       </c>
-      <c r="F5" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="G5" s="6" t="s">
+      <c r="G5" s="7" t="s">
         <v>129</v>
       </c>
       <c r="H5" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="J5">
         <v>0.95</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A6" s="6" t="s">
         <v>109</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>211</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="6"/>
+      <c r="D6" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="E6" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="E6" s="29" t="s">
+      <c r="F6" s="29" t="s">
         <v>130</v>
       </c>
-      <c r="F6" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="G6" s="6" t="s">
+      <c r="G6" s="7" t="s">
         <v>129</v>
       </c>
       <c r="H6" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="I6">
+      <c r="I6" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="J6">
         <v>0.91</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A7" s="6" t="s">
         <v>110</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>211</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="6"/>
+      <c r="D7" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="E7" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="E7" s="29" t="s">
+      <c r="F7" s="29" t="s">
         <v>130</v>
       </c>
-      <c r="F7" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="G7" s="6" t="s">
+      <c r="G7" s="7" t="s">
         <v>129</v>
       </c>
       <c r="H7" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="I7">
+      <c r="I7" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="J7">
         <v>0.91</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A8" s="6" t="s">
         <v>111</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>211</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="6"/>
+      <c r="D8" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="E8" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="E8" s="29" t="s">
+      <c r="F8" s="29" t="s">
         <v>130</v>
       </c>
-      <c r="F8" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="G8" s="6" t="s">
+      <c r="G8" s="7" t="s">
         <v>129</v>
       </c>
       <c r="H8" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="I8">
+      <c r="I8" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="J8">
         <v>0.91</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A9" s="6" t="s">
         <v>112</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="6"/>
+      <c r="D9" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="E9" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="E9" s="29" t="s">
+      <c r="F9" s="29" t="s">
         <v>130</v>
       </c>
-      <c r="F9" s="7" t="s">
+      <c r="G9" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="G9" s="6" t="s">
+      <c r="H9" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="H9" s="6" t="s">
+      <c r="I9" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="I9">
+      <c r="J9">
         <v>0.95</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A10" s="6" t="s">
         <v>113</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>214</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="6"/>
+      <c r="D10" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="E10" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="E10" s="29" t="s">
+      <c r="F10" s="29" t="s">
         <v>130</v>
       </c>
-      <c r="F10" s="7" t="s">
+      <c r="G10" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="G10" s="6" t="s">
+      <c r="H10" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="H10" s="6" t="s">
+      <c r="I10" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="I10">
+      <c r="J10">
         <v>0.95</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A11" s="6" t="s">
         <v>114</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>212</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="6"/>
+      <c r="D11" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="E11" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="E11" s="29" t="s">
+      <c r="F11" s="29" t="s">
         <v>130</v>
       </c>
-      <c r="F11" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="G11" s="6" t="s">
+      <c r="G11" s="7" t="s">
         <v>129</v>
       </c>
       <c r="H11" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="I11">
+      <c r="I11" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="J11">
         <v>0.95</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A12" s="6" t="s">
         <v>115</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="6"/>
+      <c r="D12" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="E12" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="E12" s="29" t="s">
+      <c r="F12" s="29" t="s">
         <v>130</v>
       </c>
-      <c r="F12" s="7" t="s">
+      <c r="G12" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="G12" s="6" t="s">
+      <c r="H12" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="H12" s="6" t="s">
+      <c r="I12" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="I12">
+      <c r="J12">
         <v>0.28999999999999998</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A13" s="6" t="s">
         <v>116</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="6"/>
+      <c r="D13" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="E13" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="E13" s="29" t="s">
+      <c r="F13" s="29" t="s">
         <v>130</v>
       </c>
-      <c r="F13" s="7" t="s">
+      <c r="G13" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="G13" s="6" t="s">
+      <c r="H13" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="H13" s="6" t="s">
+      <c r="I13" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="I13">
+      <c r="J13">
         <v>0.36</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A14" s="22" t="s">
         <v>117</v>
       </c>
       <c r="B14" s="22" t="s">
         <v>105</v>
       </c>
-      <c r="C14" s="22" t="s">
+      <c r="C14" s="22"/>
+      <c r="D14" s="22" t="s">
         <v>105</v>
       </c>
-      <c r="D14" s="22" t="s">
+      <c r="E14" s="22" t="s">
         <v>130</v>
       </c>
-      <c r="E14" s="29" t="s">
+      <c r="F14" s="29" t="s">
         <v>130</v>
       </c>
-      <c r="F14" s="22" t="s">
+      <c r="G14" s="22" t="s">
         <v>130</v>
       </c>
-      <c r="G14" s="22" t="s">
+      <c r="H14" s="22" t="s">
         <v>129</v>
       </c>
-      <c r="H14" s="22" t="s">
+      <c r="I14" s="22" t="s">
         <v>130</v>
       </c>
-      <c r="I14">
+      <c r="J14">
         <v>0.75</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A15" s="22" t="s">
         <v>118</v>
       </c>
       <c r="B15" s="22" t="s">
         <v>123</v>
       </c>
-      <c r="C15" s="22" t="s">
+      <c r="C15" s="22"/>
+      <c r="D15" s="22" t="s">
         <v>105</v>
       </c>
-      <c r="D15" s="22" t="s">
+      <c r="E15" s="22" t="s">
         <v>129</v>
       </c>
-      <c r="E15" s="25" t="s">
-        <v>130</v>
-      </c>
-      <c r="F15" s="22" t="s">
+      <c r="F15" s="25" t="s">
         <v>130</v>
       </c>
       <c r="G15" s="22" t="s">
         <v>130</v>
       </c>
       <c r="H15" s="22" t="s">
+        <v>130</v>
+      </c>
+      <c r="I15" s="22" t="s">
         <v>129</v>
       </c>
-      <c r="I15">
+      <c r="J15">
         <v>0.95</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A16" s="22" t="s">
         <v>215</v>
       </c>
       <c r="B16" s="22" t="s">
         <v>210</v>
       </c>
-      <c r="C16" s="22" t="s">
+      <c r="C16" s="22"/>
+      <c r="D16" s="22" t="s">
         <v>105</v>
       </c>
-      <c r="D16" s="6" t="s">
+      <c r="E16" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="E16" s="29" t="s">
+      <c r="F16" s="29" t="s">
         <v>130</v>
       </c>
-      <c r="F16" s="6" t="s">
+      <c r="G16" s="6" t="s">
         <v>130</v>
-      </c>
-      <c r="G16" s="22" t="s">
-        <v>129</v>
       </c>
       <c r="H16" s="22" t="s">
         <v>129</v>
       </c>
-      <c r="I16">
+      <c r="I16" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="J16">
         <v>0.9</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A17" s="22" t="s">
         <v>216</v>
       </c>
       <c r="B17" s="22" t="s">
         <v>209</v>
       </c>
-      <c r="C17" s="22" t="s">
+      <c r="C17" s="22"/>
+      <c r="D17" s="22" t="s">
         <v>105</v>
       </c>
-      <c r="D17" s="6" t="s">
+      <c r="E17" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="E17" s="29" t="s">
+      <c r="F17" s="29" t="s">
         <v>130</v>
       </c>
-      <c r="F17" s="6" t="s">
+      <c r="G17" s="6" t="s">
         <v>130</v>
-      </c>
-      <c r="G17" s="22" t="s">
-        <v>129</v>
       </c>
       <c r="H17" s="22" t="s">
         <v>129</v>
       </c>
-      <c r="I17">
+      <c r="I17" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="J17">
         <v>0.95</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A18" s="22" t="s">
         <v>218</v>
       </c>
       <c r="B18" s="22" t="s">
         <v>211</v>
       </c>
-      <c r="C18" s="22" t="s">
+      <c r="C18" s="22"/>
+      <c r="D18" s="22" t="s">
         <v>105</v>
       </c>
-      <c r="D18" s="6" t="s">
+      <c r="E18" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="E18" s="29" t="s">
+      <c r="F18" s="29" t="s">
         <v>130</v>
       </c>
-      <c r="F18" s="6" t="s">
+      <c r="G18" s="6" t="s">
         <v>130</v>
-      </c>
-      <c r="G18" s="22" t="s">
-        <v>129</v>
       </c>
       <c r="H18" s="22" t="s">
         <v>129</v>
       </c>
-      <c r="I18">
+      <c r="I18" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="J18">
         <v>0.95</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A19" s="22" t="s">
         <v>119</v>
       </c>
       <c r="B19" s="22" t="s">
         <v>212</v>
       </c>
-      <c r="C19" s="22" t="s">
+      <c r="C19" s="22"/>
+      <c r="D19" s="22" t="s">
         <v>105</v>
       </c>
-      <c r="D19" s="22" t="s">
+      <c r="E19" s="22" t="s">
         <v>130</v>
       </c>
-      <c r="E19" s="25" t="s">
+      <c r="F19" s="25" t="s">
         <v>130</v>
       </c>
-      <c r="F19" s="22" t="s">
+      <c r="G19" s="22" t="s">
         <v>130</v>
-      </c>
-      <c r="G19" s="22" t="s">
-        <v>129</v>
       </c>
       <c r="H19" s="22" t="s">
         <v>129</v>
       </c>
-      <c r="I19">
+      <c r="I19" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="J19">
         <v>0.95</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A20" s="22" t="s">
         <v>120</v>
       </c>
       <c r="B20" s="22" t="s">
         <v>212</v>
       </c>
-      <c r="C20" s="22" t="s">
+      <c r="C20" s="22"/>
+      <c r="D20" s="22" t="s">
         <v>105</v>
       </c>
-      <c r="D20" s="22" t="s">
+      <c r="E20" s="22" t="s">
         <v>129</v>
       </c>
-      <c r="E20" s="25" t="s">
+      <c r="F20" s="25" t="s">
         <v>130</v>
       </c>
-      <c r="F20" s="22" t="s">
+      <c r="G20" s="22" t="s">
         <v>130</v>
-      </c>
-      <c r="G20" s="22" t="s">
-        <v>129</v>
       </c>
       <c r="H20" s="22" t="s">
         <v>129</v>
       </c>
-      <c r="I20">
+      <c r="I20" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="J20">
         <v>0.91</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A21" s="22" t="s">
         <v>121</v>
       </c>
       <c r="B21" s="22" t="s">
         <v>95</v>
       </c>
-      <c r="C21" s="22" t="s">
+      <c r="C21" s="22"/>
+      <c r="D21" s="22" t="s">
         <v>105</v>
       </c>
-      <c r="D21" s="22" t="s">
+      <c r="E21" s="22" t="s">
         <v>129</v>
       </c>
-      <c r="E21" s="25" t="s">
-        <v>130</v>
-      </c>
-      <c r="F21" s="22" t="s">
+      <c r="F21" s="25" t="s">
         <v>130</v>
       </c>
       <c r="G21" s="22" t="s">
         <v>130</v>
       </c>
       <c r="H21" s="22" t="s">
+        <v>130</v>
+      </c>
+      <c r="I21" s="22" t="s">
         <v>129</v>
       </c>
-      <c r="I21">
+      <c r="J21">
         <v>0.28999999999999998</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A22" s="22" t="s">
         <v>122</v>
       </c>
       <c r="B22" s="22" t="s">
         <v>96</v>
       </c>
-      <c r="C22" s="22" t="s">
+      <c r="C22" s="22"/>
+      <c r="D22" s="22" t="s">
         <v>105</v>
       </c>
-      <c r="D22" s="22" t="s">
+      <c r="E22" s="22" t="s">
         <v>129</v>
       </c>
-      <c r="E22" s="25" t="s">
-        <v>130</v>
-      </c>
-      <c r="F22" s="22" t="s">
+      <c r="F22" s="25" t="s">
         <v>130</v>
       </c>
       <c r="G22" s="22" t="s">
         <v>130</v>
       </c>
       <c r="H22" s="22" t="s">
+        <v>130</v>
+      </c>
+      <c r="I22" s="22" t="s">
         <v>129</v>
       </c>
-      <c r="I22">
+      <c r="J22">
         <v>0.36</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A23" s="6" t="s">
         <v>131</v>
       </c>
       <c r="B23" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="C23" s="6" t="s">
+      <c r="C23" s="6"/>
+      <c r="D23" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="D23" s="6" t="s">
+      <c r="E23" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="E23" s="29" t="s">
+      <c r="F23" s="29" t="s">
         <v>130</v>
       </c>
-      <c r="F23" s="6" t="s">
+      <c r="G23" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="G23" s="6" t="s">
+      <c r="H23" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="H23" s="6" t="s">
+      <c r="I23" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="I23">
+      <c r="J23">
         <v>0.75</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A24" s="6" t="s">
         <v>132</v>
       </c>
       <c r="B24" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="C24" s="6" t="s">
+      <c r="C24" s="6"/>
+      <c r="D24" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="D24" s="6" t="s">
+      <c r="E24" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="E24" s="29" t="s">
-        <v>130</v>
-      </c>
-      <c r="F24" s="6" t="s">
+      <c r="F24" s="29" t="s">
         <v>130</v>
       </c>
       <c r="G24" s="6" t="s">
         <v>130</v>
       </c>
       <c r="H24" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="I24" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="I24">
+      <c r="J24">
         <v>0.95</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A25" s="6" t="s">
         <v>194</v>
       </c>
       <c r="B25" s="6" t="s">
         <v>212</v>
       </c>
-      <c r="C25" s="6" t="s">
+      <c r="C25" s="6"/>
+      <c r="D25" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="D25" s="6" t="s">
+      <c r="E25" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="E25" s="29" t="s">
+      <c r="F25" s="29" t="s">
         <v>130</v>
       </c>
-      <c r="F25" s="6" t="s">
+      <c r="G25" s="6" t="s">
         <v>130</v>
-      </c>
-      <c r="G25" s="6" t="s">
-        <v>129</v>
       </c>
       <c r="H25" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="I25">
+      <c r="I25" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="J25">
         <v>0.95</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A26" s="6" t="s">
         <v>133</v>
       </c>
       <c r="B26" s="6" t="s">
         <v>212</v>
       </c>
-      <c r="C26" s="6" t="s">
+      <c r="C26" s="6"/>
+      <c r="D26" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="D26" s="6" t="s">
+      <c r="E26" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="E26" s="29" t="s">
+      <c r="F26" s="29" t="s">
         <v>130</v>
       </c>
-      <c r="F26" s="6" t="s">
+      <c r="G26" s="6" t="s">
         <v>130</v>
-      </c>
-      <c r="G26" s="6" t="s">
-        <v>129</v>
       </c>
       <c r="H26" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="I26">
+      <c r="I26" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="J26">
         <v>0.95</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A27" s="6" t="s">
         <v>134</v>
       </c>
       <c r="B27" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="C27" s="6" t="s">
+      <c r="C27" s="6"/>
+      <c r="D27" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="D27" s="6" t="s">
+      <c r="E27" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="E27" s="29" t="s">
-        <v>130</v>
-      </c>
-      <c r="F27" s="6" t="s">
+      <c r="F27" s="29" t="s">
         <v>130</v>
       </c>
       <c r="G27" s="6" t="s">
         <v>130</v>
       </c>
       <c r="H27" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="I27" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="I27">
+      <c r="J27">
         <v>0.28999999999999998</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A28" s="6" t="s">
         <v>135</v>
       </c>
       <c r="B28" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="C28" s="6" t="s">
+      <c r="C28" s="6"/>
+      <c r="D28" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="D28" s="6" t="s">
+      <c r="E28" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="E28" s="29" t="s">
-        <v>130</v>
-      </c>
-      <c r="F28" s="6" t="s">
+      <c r="F28" s="29" t="s">
         <v>130</v>
       </c>
       <c r="G28" s="6" t="s">
         <v>130</v>
       </c>
       <c r="H28" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="I28" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="I28">
+      <c r="J28">
         <v>0.36</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="D3:D15 D19:D28 F19:H28 F3:H15">
+  <conditionalFormatting sqref="E3:E15 E19:E28 G19:I28 G3:I15">
     <cfRule type="cellIs" dxfId="3" priority="5" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D16:D18 F16:H18">
+  <conditionalFormatting sqref="E16:E18 G16:I18">
     <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E3:E15 E19:E28">
+  <conditionalFormatting sqref="F3:F15 F19:F28">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E16:E18">
+  <conditionalFormatting sqref="F16:F18">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"Y"</formula>
     </cfRule>

</xml_diff>